<commit_message>
Calculations of mean, standard deviation and variance of the readout noise
</commit_message>
<xml_diff>
--- a/Data/readoutNoiseDistribution_OrcaFlash4V3.xlsx
+++ b/Data/readoutNoiseDistribution_OrcaFlash4V3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/valeriepineaunoel/Documents/HiLo-Python/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{61981EDB-32E5-9B47-AAD2-4BFB57B4A408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC1F1E39-ED36-894C-B600-DC14591463AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35180" yWindow="-4860" windowWidth="28040" windowHeight="16060" xr2:uid="{EFA9A6E8-106A-F246-8D74-B7046B1734F6}"/>
+    <workbookView xWindow="-35200" yWindow="-4860" windowWidth="28040" windowHeight="16060" xr2:uid="{EFA9A6E8-106A-F246-8D74-B7046B1734F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,12 +34,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>x</t>
+    <t>readout noise [électrons]</t>
   </si>
   <si>
-    <t>y</t>
+    <t>Frequency [pixel count]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Readout info : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">mean : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">stdev : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">variance : </t>
   </si>
 </sst>
 </file>
@@ -391,51 +403,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9E76737-95C8-5E4F-A671-B6556A40C52F}">
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" customWidth="1"/>
-    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="1" max="1" width="25.83203125" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
+    <col min="5" max="6" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0.370005790387955</v>
       </c>
       <c r="B2">
         <v>2898.5507246376901</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <f>AVERAGE(A2:A43)</f>
+        <v>1.0614332588854858</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0.42096120440069401</v>
       </c>
       <c r="B3">
         <v>18357.487922705401</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <f>STDEV(A2:A43)</f>
+        <v>0.59236264225738422</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>0.45801968731905002</v>
       </c>
       <c r="B4">
         <v>33816.425120772998</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <f>E3^2</f>
+        <v>0.35089349994214974</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0.48581354950781602</v>
       </c>
@@ -443,7 +481,7 @@
         <v>105314.00966183501</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0.50897510133178803</v>
       </c>
@@ -451,7 +489,7 @@
         <v>182608.69565217401</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0.52750434279096603</v>
       </c>
@@ -459,7 +497,7 @@
         <v>234782.60869565199</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0.54603358425014403</v>
       </c>
@@ -467,7 +505,7 @@
         <v>298550.72463768098</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>0.56919513607411598</v>
       </c>
@@ -475,7 +513,7 @@
         <v>375845.41062801902</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>0.59698899826288299</v>
       </c>
@@ -483,7 +521,7 @@
         <v>455072.46376811602</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>0.61088592935726604</v>
       </c>
@@ -491,7 +529,7 @@
         <v>532367.14975845395</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>0.63867979154603305</v>
       </c>
@@ -499,7 +537,7 @@
         <v>619323.67149758397</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>0.65720903300521105</v>
       </c>
@@ -507,7 +545,7 @@
         <v>702415.45893719804</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>0.68500289519397695</v>
       </c>
@@ -515,7 +553,7 @@
         <v>785507.24637681094</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>0.70816444701794901</v>
       </c>
@@ -523,7 +561,7 @@
         <v>858937.19806763297</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>0.73132599884192195</v>
       </c>

</xml_diff>

<commit_message>
readoutNoiseDistribution.py calculation of variance, mean and standard deviation
</commit_message>
<xml_diff>
--- a/Data/readoutNoiseDistribution_OrcaFlash4V3.xlsx
+++ b/Data/readoutNoiseDistribution_OrcaFlash4V3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/valeriepineaunoel/Documents/HiLo-Python/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC1F1E39-ED36-894C-B600-DC14591463AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F31FBB-9CB4-9D40-8B24-569B423B93CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-35200" yWindow="-4860" windowWidth="28040" windowHeight="16060" xr2:uid="{EFA9A6E8-106A-F246-8D74-B7046B1734F6}"/>
   </bookViews>
@@ -406,7 +406,7 @@
   <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>